<commit_message>
Add FFC annotation processor and minor fixes
Update coverage_table signature (add forbidden_set) and ensure Ranking is cast to int in formatted names. Add process_ffc_annotations(df) to detect reused FFC IDs, remove or mark entries per parental-column rules, and append a modifications summary row. Tweak main/test routine: change default peptide/charge/test data selections, adjust loss_list/commented examples, and write output to test.xlsx sheet "4+". Add new binary file long_peptide/revised annotation.xlsx, update long_peptide/isocolumn.xlsx, remove temp ~ file and rename another temp ~ file.
</commit_message>
<xml_diff>
--- a/long_peptide/isocolumn.xlsx
+++ b/long_peptide/isocolumn.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinmbp/Desktop/2D_spec_dict/long_peptide/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A87D10-B875-5747-904B-C494E6265091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D886E19-9F3D-664D-83B1-1F988EC39EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14780" yWindow="7200" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="32400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="3+" sheetId="3" r:id="rId1"/>
     <sheet name="4+" sheetId="2" r:id="rId2"/>
-    <sheet name="3+" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1602,14 +1601,855 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="4" width="29.1640625" customWidth="1"/>
+    <col min="5" max="5" width="37.1640625" customWidth="1"/>
+    <col min="6" max="6" width="29.1640625" customWidth="1"/>
+    <col min="7" max="21" width="40.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>2</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="I1" s="2">
+        <v>-653.35199999999998</v>
+      </c>
+      <c r="J1" s="2">
+        <v>-652.851</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="L1" s="2">
+        <v>-229.11099999999999</v>
+      </c>
+      <c r="M1" s="2">
+        <v>-228.10900000000001</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="O1" s="2">
+        <v>-100.068</v>
+      </c>
+      <c r="P1" s="2">
+        <v>-99.064999999999998</v>
+      </c>
+      <c r="Q1" s="2">
+        <v>-98.042000000000002</v>
+      </c>
+      <c r="R1" s="2">
+        <v>-299.14600000000002</v>
+      </c>
+      <c r="S1" s="2">
+        <v>-216.15700000000001</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="B2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C2" t="s">
+        <v>280</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" s="2" t="s">
+        <v>282</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>280</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F4" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" t="s">
+        <v>287</v>
+      </c>
+      <c r="H4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" t="s">
+        <v>288</v>
+      </c>
+      <c r="J4" t="s">
+        <v>289</v>
+      </c>
+      <c r="N4" t="s">
+        <v>50</v>
+      </c>
+      <c r="P4" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>291</v>
+      </c>
+      <c r="R4" t="s">
+        <v>292</v>
+      </c>
+      <c r="S4" t="s">
+        <v>293</v>
+      </c>
+      <c r="T4">
+        <v>9</v>
+      </c>
+      <c r="U4" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>296</v>
+      </c>
+      <c r="F5" t="s">
+        <v>297</v>
+      </c>
+      <c r="H5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I5" t="s">
+        <v>298</v>
+      </c>
+      <c r="J5" t="s">
+        <v>299</v>
+      </c>
+      <c r="K5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>300</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="P5" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>302</v>
+      </c>
+      <c r="T5">
+        <v>7</v>
+      </c>
+      <c r="U5" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
+        <v>305</v>
+      </c>
+      <c r="F6" t="s">
+        <v>306</v>
+      </c>
+      <c r="G6" t="s">
+        <v>307</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>308</v>
+      </c>
+      <c r="N6" t="s">
+        <v>50</v>
+      </c>
+      <c r="P6" t="s">
+        <v>309</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>310</v>
+      </c>
+      <c r="T6">
+        <v>6</v>
+      </c>
+      <c r="U6" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" t="s">
+        <v>313</v>
+      </c>
+      <c r="F7" t="s">
+        <v>314</v>
+      </c>
+      <c r="G7" t="s">
+        <v>315</v>
+      </c>
+      <c r="K7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
+        <v>316</v>
+      </c>
+      <c r="M7" t="s">
+        <v>317</v>
+      </c>
+      <c r="N7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O7" t="s">
+        <v>318</v>
+      </c>
+      <c r="P7" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>320</v>
+      </c>
+      <c r="R7" t="s">
+        <v>321</v>
+      </c>
+      <c r="T7">
+        <v>9</v>
+      </c>
+      <c r="U7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" t="s">
+        <v>324</v>
+      </c>
+      <c r="M8" t="s">
+        <v>325</v>
+      </c>
+      <c r="T8">
+        <v>2</v>
+      </c>
+      <c r="U8" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>328</v>
+      </c>
+      <c r="F9" t="s">
+        <v>329</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+      <c r="L9" t="s">
+        <v>330</v>
+      </c>
+      <c r="M9" t="s">
+        <v>331</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+      <c r="O9" t="s">
+        <v>332</v>
+      </c>
+      <c r="P9" t="s">
+        <v>333</v>
+      </c>
+      <c r="R9" t="s">
+        <v>334</v>
+      </c>
+      <c r="T9">
+        <v>7</v>
+      </c>
+      <c r="U9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
+        <v>337</v>
+      </c>
+      <c r="F10" t="s">
+        <v>338</v>
+      </c>
+      <c r="K10" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" t="s">
+        <v>339</v>
+      </c>
+      <c r="M10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s">
+        <v>343</v>
+      </c>
+      <c r="F11" t="s">
+        <v>344</v>
+      </c>
+      <c r="K11" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" t="s">
+        <v>345</v>
+      </c>
+      <c r="M11" t="s">
+        <v>346</v>
+      </c>
+      <c r="N11" t="s">
+        <v>36</v>
+      </c>
+      <c r="O11" t="s">
+        <v>347</v>
+      </c>
+      <c r="T11">
+        <v>5</v>
+      </c>
+      <c r="U11" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" t="s">
+        <v>351</v>
+      </c>
+      <c r="K12" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" t="s">
+        <v>352</v>
+      </c>
+      <c r="M12" t="s">
+        <v>353</v>
+      </c>
+      <c r="N12" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" t="s">
+        <v>354</v>
+      </c>
+      <c r="P12" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>356</v>
+      </c>
+      <c r="T12">
+        <v>7</v>
+      </c>
+      <c r="U12" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B13" t="s">
+        <v>279</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
+        <v>359</v>
+      </c>
+      <c r="H13" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" t="s">
+        <v>360</v>
+      </c>
+      <c r="J13" t="s">
+        <v>361</v>
+      </c>
+      <c r="K13" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" t="s">
+        <v>362</v>
+      </c>
+      <c r="M13" t="s">
+        <v>363</v>
+      </c>
+      <c r="N13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O13" t="s">
+        <v>364</v>
+      </c>
+      <c r="P13" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>366</v>
+      </c>
+      <c r="T13">
+        <v>8</v>
+      </c>
+      <c r="U13" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" t="s">
+        <v>36</v>
+      </c>
+      <c r="L14" t="s">
+        <v>369</v>
+      </c>
+      <c r="T14">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="B15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" t="s">
+        <v>372</v>
+      </c>
+      <c r="M15" t="s">
+        <v>373</v>
+      </c>
+      <c r="T15">
+        <v>2</v>
+      </c>
+      <c r="U15" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>8</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="I16">
+        <v>3</v>
+      </c>
+      <c r="J16">
+        <v>3</v>
+      </c>
+      <c r="L16">
+        <v>9</v>
+      </c>
+      <c r="M16">
+        <v>10</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16">
+        <v>7</v>
+      </c>
+      <c r="Q16">
+        <v>6</v>
+      </c>
+      <c r="R16">
+        <v>3</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>14</v>
+      </c>
+      <c r="U16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19">
+      <c r="A17" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E17">
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>5</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="L17">
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <v>12</v>
+      </c>
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>9</v>
+      </c>
+      <c r="Q17">
+        <v>7</v>
+      </c>
+      <c r="R17">
+        <v>3</v>
+      </c>
+      <c r="S17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19">
+      <c r="A18" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19">
+      <c r="A19" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19">
+      <c r="A20" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="I20" t="s">
+        <v>375</v>
+      </c>
+      <c r="L20" t="s">
+        <v>376</v>
+      </c>
+      <c r="M20" t="s">
+        <v>377</v>
+      </c>
+      <c r="O20" t="s">
+        <v>378</v>
+      </c>
+      <c r="P20" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>380</v>
+      </c>
+      <c r="R20" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19">
+      <c r="A21" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" t="s">
+        <v>382</v>
+      </c>
+      <c r="F21" t="s">
+        <v>383</v>
+      </c>
+      <c r="S21" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19">
+      <c r="A22" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E22" t="s">
+        <v>385</v>
+      </c>
+      <c r="F22" t="s">
+        <v>386</v>
+      </c>
+      <c r="S22" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19">
+      <c r="A23" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -3235,855 +4075,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:U23"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
-  <cols>
-    <col min="1" max="6" width="29.1640625" customWidth="1"/>
-    <col min="7" max="21" width="40.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2">
-        <v>1</v>
-      </c>
-      <c r="G1" s="2">
-        <v>2</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="I1" s="2">
-        <v>-653.35199999999998</v>
-      </c>
-      <c r="J1" s="2">
-        <v>-652.851</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="L1" s="2">
-        <v>-229.11099999999999</v>
-      </c>
-      <c r="M1" s="2">
-        <v>-228.10900000000001</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="O1" s="2">
-        <v>-100.068</v>
-      </c>
-      <c r="P1" s="2">
-        <v>-99.064999999999998</v>
-      </c>
-      <c r="Q1" s="2">
-        <v>-98.042000000000002</v>
-      </c>
-      <c r="R1" s="2">
-        <v>-299.14600000000002</v>
-      </c>
-      <c r="S1" s="2">
-        <v>-216.15700000000001</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="B2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C2" t="s">
-        <v>280</v>
-      </c>
-      <c r="T2">
-        <v>0</v>
-      </c>
-      <c r="U2" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" t="s">
-        <v>280</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" t="s">
-        <v>285</v>
-      </c>
-      <c r="F4" t="s">
-        <v>286</v>
-      </c>
-      <c r="G4" t="s">
-        <v>287</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>288</v>
-      </c>
-      <c r="J4" t="s">
-        <v>289</v>
-      </c>
-      <c r="N4" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4" t="s">
-        <v>290</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>291</v>
-      </c>
-      <c r="R4" t="s">
-        <v>292</v>
-      </c>
-      <c r="S4" t="s">
-        <v>293</v>
-      </c>
-      <c r="T4">
-        <v>9</v>
-      </c>
-      <c r="U4" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" t="s">
-        <v>296</v>
-      </c>
-      <c r="F5" t="s">
-        <v>297</v>
-      </c>
-      <c r="H5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I5" t="s">
-        <v>298</v>
-      </c>
-      <c r="J5" t="s">
-        <v>299</v>
-      </c>
-      <c r="K5" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" t="s">
-        <v>300</v>
-      </c>
-      <c r="N5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>302</v>
-      </c>
-      <c r="T5">
-        <v>7</v>
-      </c>
-      <c r="U5" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="B6" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>305</v>
-      </c>
-      <c r="F6" t="s">
-        <v>306</v>
-      </c>
-      <c r="G6" t="s">
-        <v>307</v>
-      </c>
-      <c r="K6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" t="s">
-        <v>308</v>
-      </c>
-      <c r="N6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>310</v>
-      </c>
-      <c r="T6">
-        <v>6</v>
-      </c>
-      <c r="U6" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>313</v>
-      </c>
-      <c r="F7" t="s">
-        <v>314</v>
-      </c>
-      <c r="G7" t="s">
-        <v>315</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-      <c r="L7" t="s">
-        <v>316</v>
-      </c>
-      <c r="M7" t="s">
-        <v>317</v>
-      </c>
-      <c r="N7" t="s">
-        <v>50</v>
-      </c>
-      <c r="O7" t="s">
-        <v>318</v>
-      </c>
-      <c r="P7" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>320</v>
-      </c>
-      <c r="R7" t="s">
-        <v>321</v>
-      </c>
-      <c r="T7">
-        <v>9</v>
-      </c>
-      <c r="U7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>15</v>
-      </c>
-      <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="L8" t="s">
-        <v>324</v>
-      </c>
-      <c r="M8" t="s">
-        <v>325</v>
-      </c>
-      <c r="T8">
-        <v>2</v>
-      </c>
-      <c r="U8" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E9" t="s">
-        <v>328</v>
-      </c>
-      <c r="F9" t="s">
-        <v>329</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" t="s">
-        <v>330</v>
-      </c>
-      <c r="M9" t="s">
-        <v>331</v>
-      </c>
-      <c r="N9" t="s">
-        <v>36</v>
-      </c>
-      <c r="O9" t="s">
-        <v>332</v>
-      </c>
-      <c r="P9" t="s">
-        <v>333</v>
-      </c>
-      <c r="R9" t="s">
-        <v>334</v>
-      </c>
-      <c r="T9">
-        <v>7</v>
-      </c>
-      <c r="U9" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" t="s">
-        <v>337</v>
-      </c>
-      <c r="F10" t="s">
-        <v>338</v>
-      </c>
-      <c r="K10" t="s">
-        <v>50</v>
-      </c>
-      <c r="L10" t="s">
-        <v>339</v>
-      </c>
-      <c r="M10" t="s">
-        <v>340</v>
-      </c>
-      <c r="T10">
-        <v>4</v>
-      </c>
-      <c r="U10" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="2" t="s">
-        <v>342</v>
-      </c>
-      <c r="B11" t="s">
-        <v>202</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" t="s">
-        <v>343</v>
-      </c>
-      <c r="F11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K11" t="s">
-        <v>50</v>
-      </c>
-      <c r="L11" t="s">
-        <v>345</v>
-      </c>
-      <c r="M11" t="s">
-        <v>346</v>
-      </c>
-      <c r="N11" t="s">
-        <v>36</v>
-      </c>
-      <c r="O11" t="s">
-        <v>347</v>
-      </c>
-      <c r="T11">
-        <v>5</v>
-      </c>
-      <c r="U11" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="B12" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" t="s">
-        <v>350</v>
-      </c>
-      <c r="F12" t="s">
-        <v>351</v>
-      </c>
-      <c r="K12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L12" t="s">
-        <v>352</v>
-      </c>
-      <c r="M12" t="s">
-        <v>353</v>
-      </c>
-      <c r="N12" t="s">
-        <v>50</v>
-      </c>
-      <c r="O12" t="s">
-        <v>354</v>
-      </c>
-      <c r="P12" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>356</v>
-      </c>
-      <c r="T12">
-        <v>7</v>
-      </c>
-      <c r="U12" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="B13" t="s">
-        <v>279</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>359</v>
-      </c>
-      <c r="H13" t="s">
-        <v>36</v>
-      </c>
-      <c r="I13" t="s">
-        <v>360</v>
-      </c>
-      <c r="J13" t="s">
-        <v>361</v>
-      </c>
-      <c r="K13" t="s">
-        <v>50</v>
-      </c>
-      <c r="L13" t="s">
-        <v>362</v>
-      </c>
-      <c r="M13" t="s">
-        <v>363</v>
-      </c>
-      <c r="N13" t="s">
-        <v>50</v>
-      </c>
-      <c r="O13" t="s">
-        <v>364</v>
-      </c>
-      <c r="P13" t="s">
-        <v>365</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>366</v>
-      </c>
-      <c r="T13">
-        <v>8</v>
-      </c>
-      <c r="U13" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="B14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" t="s">
-        <v>369</v>
-      </c>
-      <c r="T14">
-        <v>1</v>
-      </c>
-      <c r="U14" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="B15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C15" t="s">
-        <v>15</v>
-      </c>
-      <c r="K15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" t="s">
-        <v>372</v>
-      </c>
-      <c r="M15" t="s">
-        <v>373</v>
-      </c>
-      <c r="T15">
-        <v>2</v>
-      </c>
-      <c r="U15" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="B16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16">
-        <v>9</v>
-      </c>
-      <c r="F16">
-        <v>8</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="I16">
-        <v>3</v>
-      </c>
-      <c r="J16">
-        <v>3</v>
-      </c>
-      <c r="L16">
-        <v>9</v>
-      </c>
-      <c r="M16">
-        <v>10</v>
-      </c>
-      <c r="O16">
-        <v>5</v>
-      </c>
-      <c r="P16">
-        <v>7</v>
-      </c>
-      <c r="Q16">
-        <v>6</v>
-      </c>
-      <c r="R16">
-        <v>3</v>
-      </c>
-      <c r="S16">
-        <v>1</v>
-      </c>
-      <c r="T16">
-        <v>14</v>
-      </c>
-      <c r="U16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
-      <c r="A17" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="E17">
-        <v>12</v>
-      </c>
-      <c r="F17">
-        <v>14</v>
-      </c>
-      <c r="G17">
-        <v>5</v>
-      </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>3</v>
-      </c>
-      <c r="L17">
-        <v>9</v>
-      </c>
-      <c r="M17">
-        <v>12</v>
-      </c>
-      <c r="O17">
-        <v>4</v>
-      </c>
-      <c r="P17">
-        <v>9</v>
-      </c>
-      <c r="Q17">
-        <v>7</v>
-      </c>
-      <c r="R17">
-        <v>3</v>
-      </c>
-      <c r="S17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E18">
-        <v>2</v>
-      </c>
-      <c r="F18">
-        <v>2</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>0</v>
-      </c>
-      <c r="R18">
-        <v>0</v>
-      </c>
-      <c r="S18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19">
-      <c r="A19" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19">
-      <c r="A20" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="I20" t="s">
-        <v>375</v>
-      </c>
-      <c r="L20" t="s">
-        <v>376</v>
-      </c>
-      <c r="M20" t="s">
-        <v>377</v>
-      </c>
-      <c r="O20" t="s">
-        <v>378</v>
-      </c>
-      <c r="P20" t="s">
-        <v>379</v>
-      </c>
-      <c r="Q20" t="s">
-        <v>380</v>
-      </c>
-      <c r="R20" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19">
-      <c r="A21" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="E21" t="s">
-        <v>382</v>
-      </c>
-      <c r="F21" t="s">
-        <v>383</v>
-      </c>
-      <c r="S21" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19">
-      <c r="A22" s="2" t="s">
-        <v>268</v>
-      </c>
-      <c r="E22" t="s">
-        <v>385</v>
-      </c>
-      <c r="F22" t="s">
-        <v>386</v>
-      </c>
-      <c r="S22" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="A23" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>